<commit_message>
feat: excel template with entry count
</commit_message>
<xml_diff>
--- a/templates/export/logbook.xlsx
+++ b/templates/export/logbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d050092/git/private/Socratec/traccar/templates/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043F2821-DB0F-A24E-B5E2-05BB0CF35798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FFE68C-A4A1-1E4B-A89C-11611ACEE914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="31020" windowHeight="13380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="31020" windowHeight="13380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>jx:area(lastCell="N9")</t>
+          <t>jx:area(lastCell="N11")</t>
         </r>
       </text>
     </comment>
@@ -52,12 +52,11 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="devices", var="device", lastCell="N9" multisheet="sheetNames")
-</t>
+          <t>jx:each(items="devices", var="device", lastCell="N11" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +65,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="entry", lastCell="N9")</t>
+          <t>jx:each(items="device.objects", var="entry", lastCell="N11")</t>
         </r>
       </text>
     </comment>
@@ -75,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Report type:</t>
   </si>
@@ -183,6 +182,15 @@
   </si>
   <si>
     <t>${entry.notes}</t>
+  </si>
+  <si>
+    <t>${device.objects.size()}</t>
+  </si>
+  <si>
+    <t>Entries:</t>
+  </si>
+  <si>
+    <t>Distance:</t>
   </si>
 </sst>
 </file>
@@ -456,7 +464,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>2418840</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>53570</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -513,7 +521,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>2418840</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>53570</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -570,7 +578,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>2418840</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>53570</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -795,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1000"/>
+  <dimension ref="A1:N1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -913,12 +921,16 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="8"/>
+    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -926,96 +938,122 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:14" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="M10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="N10" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+    <row r="11" spans="1:14" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I11" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K11" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="M11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="15" t="s">
+      <c r="N11" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1994,6 +2032,8 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
feat: add total distance in excel export
</commit_message>
<xml_diff>
--- a/templates/export/logbook.xlsx
+++ b/templates/export/logbook.xlsx
@@ -8,15 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d050092/git/private/Socratec/traccar/templates/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FFE68C-A4A1-1E4B-A89C-11611ACEE914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D6E00B-AA5A-4A47-85EC-B694472E1019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="31020" windowHeight="13380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -74,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Report type:</t>
   </si>
@@ -191,6 +202,9 @@
   </si>
   <si>
     <t>Distance:</t>
+  </si>
+  <si>
+    <t>${distanceUnit.equals("mi") ? "".format("%.1f mi", device.totalDistance * 0.000621371) : distanceUnit.equals("nmi") ? "".format("%.1f nmi", device.totalDistance * 0.000539957) : "".format("%.1f km", device.totalDistance * 0.001)}</t>
   </si>
 </sst>
 </file>
@@ -806,7 +820,7 @@
   <dimension ref="A1:N1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -938,11 +952,13 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="8"/>

</xml_diff>

<commit_message>
feat: add sums to excel trip reporting
</commit_message>
<xml_diff>
--- a/templates/export/logbook.xlsx
+++ b/templates/export/logbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d050092/git/private/Socratec/traccar/templates/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D6E00B-AA5A-4A47-85EC-B694472E1019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F035C2C5-8894-4F45-AE16-8227AF17FF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="31020" windowHeight="13380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>jx:area(lastCell="N11")</t>
+          <t>jx:area(lastCell="N13")</t>
         </r>
       </text>
     </comment>
@@ -63,11 +63,11 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="devices", var="device", lastCell="N11" multisheet="sheetNames")</t>
+          <t>jx:each(items="devices", var="device", lastCell="N13" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="entry", lastCell="N11")</t>
+          <t>jx:each(items="device.objects", var="entry", lastCell="N13")</t>
         </r>
       </text>
     </comment>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Report type:</t>
   </si>
@@ -201,10 +201,40 @@
     <t>Entries:</t>
   </si>
   <si>
-    <t>Distance:</t>
+    <t>Distance total:</t>
+  </si>
+  <si>
+    <t>Distance private</t>
+  </si>
+  <si>
+    <t>Distance business</t>
+  </si>
+  <si>
+    <t>Duration total</t>
+  </si>
+  <si>
+    <t>Duration private</t>
+  </si>
+  <si>
+    <t>Duration business</t>
   </si>
   <si>
     <t>${distanceUnit.equals("mi") ? "".format("%.1f mi", device.totalDistance * 0.000621371) : distanceUnit.equals("nmi") ? "".format("%.1f nmi", device.totalDistance * 0.000539957) : "".format("%.1f km", device.totalDistance * 0.001)}</t>
+  </si>
+  <si>
+    <t>${distanceUnit.equals("mi") ? "".format("%.1f mi", device.privateDistance * 0.000621371) : distanceUnit.equals("nmi") ? "".format("%.1f nmi", device.privateDistance * 0.000539957) : "".format("%.1f km", device.privateDistance * 0.001)}</t>
+  </si>
+  <si>
+    <t>${distanceUnit.equals("mi") ? "".format("%.1f mi", device.businessDistance * 0.000621371) : distanceUnit.equals("nmi") ? "".format("%.1f nmi", device.businessDistance * 0.000539957) : "".format("%.1f km", device.businessDistance * 0.001)}</t>
+  </si>
+  <si>
+    <t>${device.totalDuration/86400000.0}</t>
+  </si>
+  <si>
+    <t>${device.privateDuration/86400000.0}</t>
+  </si>
+  <si>
+    <t>${device.businessDuration/86400000.0}</t>
   </si>
 </sst>
 </file>
@@ -478,7 +508,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>2418840</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>53570</xdr:rowOff>
+      <xdr:rowOff>21820</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -535,7 +565,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>2418840</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>53570</xdr:rowOff>
+      <xdr:rowOff>21820</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -592,7 +622,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>2418840</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>53570</xdr:rowOff>
+      <xdr:rowOff>21820</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -817,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1002"/>
+  <dimension ref="A1:N1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -943,7 +973,7 @@
         <v>36</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="8"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -957,11 +987,15 @@
         <v>38</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="8"/>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>47</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -969,12 +1003,20 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="8"/>
+    <row r="9" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -982,96 +1024,128 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:14" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="M12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="N12" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+    <row r="13" spans="1:14" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I13" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M13" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="15" t="s">
+      <c r="N13" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2050,6 +2124,8 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
feat: add sums to excel trip reporting (#8)
Co-authored-by: Riegel, Steven <>
</commit_message>
<xml_diff>
--- a/templates/export/logbook.xlsx
+++ b/templates/export/logbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d050092/git/private/Socratec/traccar/templates/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D6E00B-AA5A-4A47-85EC-B694472E1019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F035C2C5-8894-4F45-AE16-8227AF17FF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="31020" windowHeight="13380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>jx:area(lastCell="N11")</t>
+          <t>jx:area(lastCell="N13")</t>
         </r>
       </text>
     </comment>
@@ -63,11 +63,11 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="devices", var="device", lastCell="N11" multisheet="sheetNames")</t>
+          <t>jx:each(items="devices", var="device", lastCell="N13" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="entry", lastCell="N11")</t>
+          <t>jx:each(items="device.objects", var="entry", lastCell="N13")</t>
         </r>
       </text>
     </comment>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Report type:</t>
   </si>
@@ -201,10 +201,40 @@
     <t>Entries:</t>
   </si>
   <si>
-    <t>Distance:</t>
+    <t>Distance total:</t>
+  </si>
+  <si>
+    <t>Distance private</t>
+  </si>
+  <si>
+    <t>Distance business</t>
+  </si>
+  <si>
+    <t>Duration total</t>
+  </si>
+  <si>
+    <t>Duration private</t>
+  </si>
+  <si>
+    <t>Duration business</t>
   </si>
   <si>
     <t>${distanceUnit.equals("mi") ? "".format("%.1f mi", device.totalDistance * 0.000621371) : distanceUnit.equals("nmi") ? "".format("%.1f nmi", device.totalDistance * 0.000539957) : "".format("%.1f km", device.totalDistance * 0.001)}</t>
+  </si>
+  <si>
+    <t>${distanceUnit.equals("mi") ? "".format("%.1f mi", device.privateDistance * 0.000621371) : distanceUnit.equals("nmi") ? "".format("%.1f nmi", device.privateDistance * 0.000539957) : "".format("%.1f km", device.privateDistance * 0.001)}</t>
+  </si>
+  <si>
+    <t>${distanceUnit.equals("mi") ? "".format("%.1f mi", device.businessDistance * 0.000621371) : distanceUnit.equals("nmi") ? "".format("%.1f nmi", device.businessDistance * 0.000539957) : "".format("%.1f km", device.businessDistance * 0.001)}</t>
+  </si>
+  <si>
+    <t>${device.totalDuration/86400000.0}</t>
+  </si>
+  <si>
+    <t>${device.privateDuration/86400000.0}</t>
+  </si>
+  <si>
+    <t>${device.businessDuration/86400000.0}</t>
   </si>
 </sst>
 </file>
@@ -478,7 +508,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>2418840</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>53570</xdr:rowOff>
+      <xdr:rowOff>21820</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -535,7 +565,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>2418840</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>53570</xdr:rowOff>
+      <xdr:rowOff>21820</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -592,7 +622,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>2418840</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>53570</xdr:rowOff>
+      <xdr:rowOff>21820</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -817,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1002"/>
+  <dimension ref="A1:N1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -943,7 +973,7 @@
         <v>36</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="8"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -957,11 +987,15 @@
         <v>38</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="8"/>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>47</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -969,12 +1003,20 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="8"/>
+    <row r="9" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -982,96 +1024,128 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:14" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="M12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="N12" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+    <row r="13" spans="1:14" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I13" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M13" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="15" t="s">
+      <c r="N13" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2050,6 +2124,8 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>